<commit_message>
Ajustes no banco de dados e carregamento dos dados históricos.
</commit_message>
<xml_diff>
--- a/Doc referencia/Conta Contabil.xlsx
+++ b/Doc referencia/Conta Contabil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aplicativos Desenvolvidos\dashboard_financeiro\Doc referencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14547C37-5E46-4FED-99EB-B4AFAFC03479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81C52FF-5D89-444F-8C37-7D829B052BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{25D6BD5D-DF33-4417-BE38-FA53BFEE0241}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{25D6BD5D-DF33-4417-BE38-FA53BFEE0241}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -1004,7 +1004,7 @@
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{52289F67-5371-4774-B686-631B8173DE36}" name="CÓDIGO CONTA CONTÁBIL" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{35003519-F52E-4615-ABC7-DFF35C43358F}" name="DESCRIÇÃO CONTA CONTÁBIL" dataDxfId="0" dataCellStyle="Porcentagem"/>
+    <tableColumn id="2" xr3:uid="{35003519-F52E-4615-ABC7-DFF35C43358F}" name="DESCRIÇÃO CONTA CONTÁBIL" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1330,7 +1330,7 @@
   <dimension ref="A1:B372"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4563,20 +4563,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d3612971-7074-4360-9f87-cc78d3d5baf3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d3612971-7074-4360-9f87-cc78d3d5baf3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4599,14 +4599,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E0999EF-4D6B-4F27-93DA-F180519AD666}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{389FE0E0-260D-4916-B338-3655505DCA45}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -4623,6 +4615,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E0999EF-4D6B-4F27-93DA-F180519AD666}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{0a9b9e15-83d2-4075-9282-a04e05c6580a}" enabled="1" method="Standard" siteId="{24139d14-c62c-4c47-8bdd-ce71ea1d50cf}" removed="0"/>

</xml_diff>